<commit_message>
Se hicieron ajustes minimos
</commit_message>
<xml_diff>
--- a/ESPECIALIDADES.xlsx
+++ b/ESPECIALIDADES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erincon/Desktop/codigo-sofi/script-para-migrar-nuevas-especialidades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE87A3EC-E589-B84F-964C-4A23BFC2404B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DECB49-1F73-6E4B-8710-B3E0411934C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EQUIVALENCIAS" sheetId="1" r:id="rId1"/>
@@ -389,63 +389,42 @@
     <t xml:space="preserve"> RESIDENCIA                              </t>
   </si>
   <si>
-    <t xml:space="preserve"> NEFROLOGÍA                              </t>
-  </si>
-  <si>
     <t>NEF</t>
   </si>
   <si>
     <t>NEFROLOGIA</t>
   </si>
   <si>
-    <t xml:space="preserve"> NEFROLOGÍA PEDIÁTRICA                   </t>
-  </si>
-  <si>
     <t>NFP</t>
   </si>
   <si>
     <t>NEFROLOGIA PEDIATRICA</t>
   </si>
   <si>
-    <t xml:space="preserve"> NEUMOLOGÍA                              </t>
-  </si>
-  <si>
     <t>NEUM</t>
   </si>
   <si>
     <t>NEUMOLOGIA</t>
   </si>
   <si>
-    <t xml:space="preserve"> NEUROCIRUGÍA                            </t>
-  </si>
-  <si>
     <t>NEC</t>
   </si>
   <si>
     <t>NEUROCIRUGIA</t>
   </si>
   <si>
-    <t xml:space="preserve"> NEUROLOGÍA                              </t>
-  </si>
-  <si>
     <t>NEUR</t>
   </si>
   <si>
     <t>NEUROLOGIA</t>
   </si>
   <si>
-    <t xml:space="preserve"> NEURO PEDIATRÍA                         </t>
-  </si>
-  <si>
     <t>NEP</t>
   </si>
   <si>
     <t>NEUROLOGIA PEDIATRICA</t>
   </si>
   <si>
-    <t xml:space="preserve"> NUTRICIÓN                               </t>
-  </si>
-  <si>
     <t>NUT</t>
   </si>
   <si>
@@ -461,63 +440,33 @@
     <t>ODONTOLOGIA</t>
   </si>
   <si>
-    <t xml:space="preserve"> OFTALMOLOGÍA                            </t>
-  </si>
-  <si>
     <t>OFT</t>
   </si>
   <si>
     <t>OFTALMOLOGIA</t>
   </si>
   <si>
-    <t xml:space="preserve"> ONCOLOGÍA                               </t>
-  </si>
-  <si>
     <t>ONC</t>
   </si>
   <si>
     <t>ONCOLOGIA</t>
   </si>
   <si>
-    <t xml:space="preserve"> ONCOLOGÍA MÉDICA                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ONCOLOGÍA RADIACIÓN                     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CIRUGÍA ORTOPÉDICA                      </t>
-  </si>
-  <si>
     <t>ORT</t>
   </si>
   <si>
     <t>ORTOPEDIA Y TRAUMATOLOGIA</t>
   </si>
   <si>
-    <t xml:space="preserve"> ORTOPEDÍA TRAUMATOLÓGICA                </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> OTORRINOLARINGOLOGÍA                    </t>
-  </si>
-  <si>
     <t>OTO</t>
   </si>
   <si>
     <t>OTORRINOLARINGOLOGIA</t>
   </si>
   <si>
-    <t xml:space="preserve"> CIRUGÍA CABEZA Y CUELLO                 </t>
-  </si>
-  <si>
     <t>OTORRINOLARINGOLOGIA Y CIRUGIA DE CABEZA Y CUELLO</t>
   </si>
   <si>
-    <t xml:space="preserve"> CIRUGÍA ORAL Y MAXILOFACIAL             </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ADMINISTRATIVO                          </t>
-  </si>
-  <si>
     <t>OTRO</t>
   </si>
   <si>
@@ -563,9 +512,6 @@
     <t xml:space="preserve"> PLAN FARMACIA                           </t>
   </si>
   <si>
-    <t xml:space="preserve"> VIH/SIDA                                </t>
-  </si>
-  <si>
     <t xml:space="preserve"> OTRA ESPECIALIDAD CLÍNICA               </t>
   </si>
   <si>
@@ -854,9 +800,6 @@
     <t xml:space="preserve"> CARDIOLOGÍA, GENERAL</t>
   </si>
   <si>
-    <t xml:space="preserve"> CARDIOLOGÍA, ECOCARDIOLOGÍA</t>
-  </si>
-  <si>
     <t xml:space="preserve"> CARDIOLOGÍA, ELECTROFISIOLOGÍA</t>
   </si>
   <si>
@@ -882,6 +825,63 @@
   </si>
   <si>
     <t>RESIDENTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CARDIOLOGÍA, ECOCARGIOLOGÍA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NEFROLOGÍA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NEFROLOGÍA PEDIÁTRICA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NEUMOLOGÍA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NEUROCIRUGÍA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NEURO PEDIATRÍA </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NUTRICIÓN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ONCOLOGÍA MÉDICA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ONCOLOGÍA RADIACIÓN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CIRUGÍA ORTOPÉDICA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ORTOPEDÍA TRAUMATOLÓGICA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OTORRINOLARINGOLOGÍA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CIRUGÍA CABEZA Y CUELLO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CIRUGÍA ORAL Y MAXILOFACIAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ADMINISTRATIVO </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> VIH/SIDA</t>
   </si>
 </sst>
 </file>
@@ -1252,8 +1252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C115"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1352,7 +1352,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -1363,7 +1363,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
@@ -1374,7 +1374,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>275</v>
+        <v>256</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
@@ -1550,7 +1550,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>276</v>
+        <v>257</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>45</v>
@@ -1935,596 +1935,596 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>266</v>
+      </c>
+      <c r="B62" t="s">
         <v>119</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
         <v>120</v>
-      </c>
-      <c r="C62" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>267</v>
+      </c>
+      <c r="B63" t="s">
+        <v>121</v>
+      </c>
+      <c r="C63" t="s">
         <v>122</v>
-      </c>
-      <c r="B63" t="s">
-        <v>123</v>
-      </c>
-      <c r="C63" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>125</v>
+        <v>268</v>
       </c>
       <c r="B64" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C64" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>128</v>
+        <v>269</v>
       </c>
       <c r="B65" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C65" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>131</v>
+        <v>270</v>
       </c>
       <c r="B66" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C66" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>134</v>
+        <v>271</v>
       </c>
       <c r="B67" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C67" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>137</v>
+        <v>272</v>
       </c>
       <c r="B68" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C68" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B69" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C69" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>143</v>
+        <v>273</v>
       </c>
       <c r="B70" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C70" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>146</v>
+        <v>274</v>
       </c>
       <c r="B71" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C71" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>149</v>
+        <v>275</v>
       </c>
       <c r="B72" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C72" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>150</v>
+        <v>276</v>
       </c>
       <c r="B73" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C73" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>280</v>
+        <v>261</v>
       </c>
       <c r="B74" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C74" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>151</v>
+        <v>277</v>
       </c>
       <c r="B75" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="C75" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>154</v>
+        <v>278</v>
       </c>
       <c r="B76" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="C76" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>155</v>
+        <v>279</v>
       </c>
       <c r="B77" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="C77" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>158</v>
+        <v>280</v>
       </c>
       <c r="B78" t="s">
         <v>32</v>
       </c>
       <c r="C78" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>160</v>
+        <v>281</v>
       </c>
       <c r="B79" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="C79" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>161</v>
+        <v>282</v>
       </c>
       <c r="B80" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="C80" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="B81" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="C81" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="B82" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="C82" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="B83" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="C83" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="B84" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="C84" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="B85" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="C85" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="B86" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="C86" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="B87" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="C87" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="B88" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="C88" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="B89" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="C89" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="B90" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="C90" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="B91" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="C91" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="B92" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="C92" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="B93" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="C93" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>177</v>
+        <v>283</v>
       </c>
       <c r="B94" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="C94" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="B95" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="C95" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="B96" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="C96" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="B97" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="C97" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
       <c r="B98" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="C98" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="B99" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="C99" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="B100" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="C100" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="B101" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="C101" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="B102" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="C102" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
       <c r="B103" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="C103" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="B104" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="C104" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="B105" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="C105" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>277</v>
+        <v>258</v>
       </c>
       <c r="B106" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="C106" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="B107" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="C107" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="B108" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="C108" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="B109" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="C109" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
       <c r="B110" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="C110" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="B111" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="C111" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="B112" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="C112" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="B113" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="C113" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="B114" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="C114" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>278</v>
+        <v>259</v>
       </c>
       <c r="B115" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C115" t="s">
-        <v>279</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -2538,7 +2538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
@@ -2554,7 +2554,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -2567,10 +2567,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="B3" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2591,15 +2591,15 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="B6" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
@@ -2631,18 +2631,18 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="B11" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="B12" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -2703,10 +2703,10 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="B20" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -2719,10 +2719,10 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="B22" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -2751,159 +2751,159 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B26" t="s">
         <v>120</v>
-      </c>
-      <c r="B26" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B27" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B28" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B29" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B30" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B31" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B32" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B33" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="B34" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="B35" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="B36" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="B37" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="B38" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="B39" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="B40" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="B41" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="B42" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="B43" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="B44" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="B45" t="s">
         <v>22</v>
@@ -2911,10 +2911,10 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="B46" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -2935,18 +2935,18 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="B49" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="B50" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -2962,7 +2962,7 @@
         <v>21</v>
       </c>
       <c r="B52" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -2978,7 +2978,7 @@
         <v>100</v>
       </c>
       <c r="B54" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -3023,18 +3023,18 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="B60" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="B61" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -3047,98 +3047,98 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B63" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="B64" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B65" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="B66" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="B67" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="B68" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="B69" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="B70" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="B71" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="B72" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="B73" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="B74" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
@@ -3151,10 +3151,10 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="B76" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
@@ -3162,71 +3162,71 @@
         <v>110</v>
       </c>
       <c r="B77" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="B78" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="B79" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
       <c r="B80" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
       <c r="B81" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="B82" t="s">
-        <v>269</v>
+        <v>251</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="B83" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="B84" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>282</v>
+        <v>263</v>
       </c>
       <c r="B85" t="s">
-        <v>283</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>